<commit_message>
Added entry screen for supervision
</commit_message>
<xml_diff>
--- a/app/config/tables/SUPERVISIONHC/Forms/SUPERVISIONHC/SUPERVISIONHC.xlsx
+++ b/app/config/tables/SUPERVISIONHC/Forms/SUPERVISIONHC/SUPERVISIONHC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFB5A4C-FB74-4587-B48D-77F187527C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97EC906-28E9-405A-880D-5A208799FDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="351">
   <si>
     <t>setting_name</t>
   </si>
@@ -261,12 +261,6 @@
     <t>Assistants</t>
   </si>
   <si>
-    <t>SUPERVISOR</t>
-  </si>
-  <si>
-    <t>Supervisor</t>
-  </si>
-  <si>
     <t>select_one</t>
   </si>
   <si>
@@ -1045,6 +1039,54 @@
   </si>
   <si>
     <t>AJ Vaccines A/S: Data de validade do solvente</t>
+  </si>
+  <si>
+    <t>ASSISTANT</t>
+  </si>
+  <si>
+    <t>Assistant</t>
+  </si>
+  <si>
+    <t>Assistente</t>
+  </si>
+  <si>
+    <t>HCAREA</t>
+  </si>
+  <si>
+    <t>REG</t>
+  </si>
+  <si>
+    <t>VISITDATE</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>HCAREANOME</t>
+  </si>
+  <si>
+    <t>REGNOME</t>
+  </si>
+  <si>
+    <t>You are about to supervise at:</t>
+  </si>
+  <si>
+    <t>Você está prestes a supervisionar em:</t>
+  </si>
+  <si>
+    <t>Region: &lt;b&gt;{{data.REGNOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Região: &lt;b&gt;{{data.REGNOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Health centre area: &lt;b&gt;{{data.HCAREANOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Área sanitárias: &lt;b&gt;{{data.HCAREANOME}}&lt;/b&gt;</t>
   </si>
 </sst>
 </file>
@@ -1580,11 +1622,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:T159"/>
+  <dimension ref="A1:T163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,664 +1719,671 @@
       <c r="B2" t="s">
         <v>37</v>
       </c>
+      <c r="R2" s="10"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>345</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="R3" s="10"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>347</v>
+      </c>
+      <c r="H4" t="s">
+        <v>348</v>
+      </c>
+      <c r="R4" s="10"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>349</v>
+      </c>
+      <c r="H5" t="s">
+        <v>350</v>
+      </c>
+      <c r="R5" s="10"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>335</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
+        <v>336</v>
       </c>
       <c r="H6" t="s">
-        <v>87</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s">
-        <v>81</v>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>340</v>
+      </c>
+      <c r="G7" t="s">
+        <v>341</v>
+      </c>
+      <c r="H7" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H8" t="s">
-        <v>84</v>
-      </c>
-      <c r="R8" s="19"/>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>98</v>
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11" t="s">
-        <v>252</v>
-      </c>
-      <c r="G11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H11" t="s">
-        <v>103</v>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" t="s">
+        <v>82</v>
+      </c>
+      <c r="R12" s="19"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H14" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>38</v>
+      <c r="D15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" t="s">
+        <v>250</v>
+      </c>
+      <c r="G15" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" t="s">
-        <v>113</v>
-      </c>
-      <c r="G17" t="s">
-        <v>114</v>
-      </c>
-      <c r="H17" t="s">
-        <v>115</v>
-      </c>
-    </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>38</v>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" t="s">
-        <v>163</v>
-      </c>
-      <c r="G20" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" t="s">
-        <v>117</v>
-      </c>
-    </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" t="s">
-        <v>164</v>
+      <c r="D21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" t="s">
+        <v>112</v>
+      </c>
+      <c r="H21" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" t="s">
-        <v>165</v>
-      </c>
-      <c r="G22" t="s">
-        <v>118</v>
-      </c>
-      <c r="H22" t="s">
-        <v>253</v>
+      <c r="B22" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" t="s">
-        <v>166</v>
-      </c>
-      <c r="G23" t="s">
-        <v>119</v>
-      </c>
-      <c r="H23" t="s">
-        <v>254</v>
+      <c r="B23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
       </c>
       <c r="F24" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G24" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H24" t="s">
-        <v>255</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="F26" t="s">
-        <v>289</v>
+        <v>163</v>
       </c>
       <c r="G26" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H26" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>45</v>
+        <v>75</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
       </c>
       <c r="F27" t="s">
-        <v>290</v>
+        <v>164</v>
       </c>
       <c r="G27" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H27" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>45</v>
+        <v>75</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>291</v>
+        <v>165</v>
       </c>
       <c r="G28" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H28" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>85</v>
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>127</v>
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" t="s">
+        <v>287</v>
+      </c>
+      <c r="G30" t="s">
+        <v>119</v>
+      </c>
+      <c r="H30" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>38</v>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" t="s">
+        <v>288</v>
+      </c>
+      <c r="G31" t="s">
+        <v>120</v>
+      </c>
+      <c r="H31" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" t="s">
-        <v>164</v>
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" t="s">
+        <v>289</v>
+      </c>
+      <c r="G32" t="s">
+        <v>121</v>
+      </c>
+      <c r="H32" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="H34" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>98</v>
-      </c>
-      <c r="F35" t="s">
-        <v>169</v>
-      </c>
-      <c r="G35" t="s">
-        <v>129</v>
-      </c>
-      <c r="H35" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>98</v>
-      </c>
-      <c r="F36" t="s">
-        <v>170</v>
-      </c>
-      <c r="G36" t="s">
-        <v>132</v>
-      </c>
-      <c r="H36" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>98</v>
-      </c>
-      <c r="F37" t="s">
-        <v>171</v>
-      </c>
-      <c r="G37" t="s">
-        <v>130</v>
-      </c>
-      <c r="H37" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>98</v>
-      </c>
-      <c r="F38" t="s">
-        <v>172</v>
-      </c>
-      <c r="G38" t="s">
-        <v>133</v>
+        <v>35</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>126</v>
       </c>
       <c r="H38" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F39" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H39" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F40" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G40" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H40" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>38</v>
+      <c r="D41" t="s">
+        <v>96</v>
+      </c>
+      <c r="F41" t="s">
+        <v>169</v>
+      </c>
+      <c r="G41" t="s">
+        <v>128</v>
+      </c>
+      <c r="H41" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>37</v>
+      <c r="D42" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" t="s">
+        <v>170</v>
+      </c>
+      <c r="G42" t="s">
+        <v>131</v>
+      </c>
+      <c r="H42" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>77</v>
-      </c>
-      <c r="E43" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="F43" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G43" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H43" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="F44" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G44" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H44" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F45" t="s">
-        <v>177</v>
-      </c>
-      <c r="G45" t="s">
-        <v>137</v>
-      </c>
-      <c r="H45" t="s">
-        <v>268</v>
+      <c r="B45" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>75</v>
+      </c>
+      <c r="E47" t="s">
         <v>47</v>
       </c>
-      <c r="F46" t="s">
-        <v>178</v>
-      </c>
-      <c r="G46" t="s">
-        <v>138</v>
-      </c>
-      <c r="H46" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>80</v>
-      </c>
-      <c r="C47" t="s">
-        <v>179</v>
+      <c r="F47" t="s">
+        <v>173</v>
+      </c>
+      <c r="G47" t="s">
+        <v>133</v>
+      </c>
+      <c r="H47" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="F48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G48" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H48" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>77</v>
-      </c>
-      <c r="E49" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" t="s">
+        <v>175</v>
+      </c>
+      <c r="G49" t="s">
+        <v>135</v>
+      </c>
+      <c r="H49" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50" t="s">
         <v>47</v>
       </c>
-      <c r="F49" t="s">
-        <v>181</v>
-      </c>
-      <c r="G49" t="s">
-        <v>140</v>
-      </c>
-      <c r="H49" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>85</v>
+      <c r="F50" t="s">
+        <v>176</v>
+      </c>
+      <c r="G50" t="s">
+        <v>136</v>
+      </c>
+      <c r="H50" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>38</v>
+        <v>78</v>
+      </c>
+      <c r="C51" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>85</v>
+      <c r="D52" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" t="s">
+        <v>178</v>
+      </c>
+      <c r="G52" t="s">
+        <v>137</v>
+      </c>
+      <c r="H52" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>37</v>
+      <c r="D53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" t="s">
+        <v>47</v>
+      </c>
+      <c r="F53" t="s">
+        <v>179</v>
+      </c>
+      <c r="G53" t="s">
+        <v>138</v>
+      </c>
+      <c r="H53" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
-        <v>77</v>
-      </c>
-      <c r="E54" t="s">
-        <v>47</v>
-      </c>
-      <c r="F54" t="s">
-        <v>142</v>
-      </c>
-      <c r="G54" t="s">
-        <v>141</v>
-      </c>
-      <c r="H54" t="s">
-        <v>272</v>
+      <c r="B54" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>80</v>
-      </c>
-      <c r="C55" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
-        <v>45</v>
-      </c>
-      <c r="F56" t="s">
-        <v>145</v>
-      </c>
-      <c r="G56" t="s">
-        <v>146</v>
-      </c>
-      <c r="H56" t="s">
-        <v>273</v>
+      <c r="B56" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>80</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
+        <v>75</v>
+      </c>
+      <c r="E58" t="s">
+        <v>47</v>
+      </c>
+      <c r="F58" t="s">
+        <v>140</v>
+      </c>
+      <c r="G58" t="s">
+        <v>139</v>
+      </c>
+      <c r="H58" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60" t="s">
+        <v>143</v>
+      </c>
+      <c r="G60" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>77</v>
-      </c>
-      <c r="E59" t="s">
-        <v>47</v>
-      </c>
-      <c r="F59" t="s">
-        <v>148</v>
-      </c>
-      <c r="G59" t="s">
-        <v>147</v>
-      </c>
-      <c r="H59" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>80</v>
-      </c>
-      <c r="C60" t="s">
-        <v>149</v>
+      <c r="H60" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>45</v>
-      </c>
-      <c r="F61" t="s">
-        <v>150</v>
-      </c>
-      <c r="G61" t="s">
-        <v>151</v>
-      </c>
-      <c r="H61" t="s">
-        <v>275</v>
+      <c r="B61" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>85</v>
+        <v>78</v>
+      </c>
+      <c r="C62" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E63" t="s">
         <v>47</v>
       </c>
       <c r="F63" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="G63" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="H63" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C64" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
@@ -2342,10 +2391,10 @@
         <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G65" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="H65" t="s">
         <v>273</v>
@@ -2353,160 +2402,148 @@
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>80</v>
-      </c>
-      <c r="C67" t="s">
-        <v>155</v>
+      <c r="D67" t="s">
+        <v>75</v>
+      </c>
+      <c r="E67" t="s">
+        <v>47</v>
+      </c>
+      <c r="F67" t="s">
+        <v>150</v>
+      </c>
+      <c r="G67" t="s">
+        <v>151</v>
+      </c>
+      <c r="H67" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>77</v>
-      </c>
-      <c r="E68" t="s">
-        <v>47</v>
-      </c>
-      <c r="F68" t="s">
-        <v>157</v>
-      </c>
-      <c r="G68" t="s">
-        <v>158</v>
-      </c>
-      <c r="H68" t="s">
-        <v>277</v>
+      <c r="B68" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>80</v>
-      </c>
-      <c r="C69" t="s">
-        <v>159</v>
+      <c r="D69" t="s">
+        <v>45</v>
+      </c>
+      <c r="F69" t="s">
+        <v>154</v>
+      </c>
+      <c r="G69" t="s">
+        <v>119</v>
+      </c>
+      <c r="H69" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
-        <v>45</v>
-      </c>
-      <c r="F70" t="s">
-        <v>160</v>
-      </c>
-      <c r="G70" t="s">
-        <v>161</v>
-      </c>
-      <c r="H70" t="s">
-        <v>278</v>
+      <c r="B70" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>85</v>
+        <v>78</v>
+      </c>
+      <c r="C71" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>85</v>
+      <c r="D72" t="s">
+        <v>75</v>
+      </c>
+      <c r="E72" t="s">
+        <v>47</v>
+      </c>
+      <c r="F72" t="s">
+        <v>155</v>
+      </c>
+      <c r="G72" t="s">
+        <v>156</v>
+      </c>
+      <c r="H72" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>85</v>
+        <v>78</v>
+      </c>
+      <c r="C73" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>38</v>
+      <c r="D74" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" t="s">
+        <v>158</v>
+      </c>
+      <c r="G74" t="s">
+        <v>159</v>
+      </c>
+      <c r="H74" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
-        <v>35</v>
-      </c>
-      <c r="G76" t="s">
-        <v>162</v>
-      </c>
-      <c r="H76" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
-        <v>112</v>
-      </c>
-      <c r="F77" t="s">
-        <v>182</v>
-      </c>
-      <c r="G77" t="s">
-        <v>305</v>
-      </c>
-      <c r="H77" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D78" t="s">
-        <v>28</v>
-      </c>
-      <c r="F78" t="s">
-        <v>183</v>
-      </c>
-      <c r="G78" t="s">
-        <v>306</v>
-      </c>
-      <c r="H78" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
-        <v>112</v>
-      </c>
-      <c r="F79" t="s">
-        <v>184</v>
-      </c>
-      <c r="G79" t="s">
-        <v>307</v>
-      </c>
-      <c r="H79" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
-        <v>28</v>
-      </c>
-      <c r="F80" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="G80" t="s">
-        <v>308</v>
+        <v>160</v>
       </c>
       <c r="H80" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F81" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G81" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="H81" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
@@ -2514,27 +2551,27 @@
         <v>28</v>
       </c>
       <c r="F82" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G82" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="H82" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F83" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G83" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="H83" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
@@ -2542,104 +2579,104 @@
         <v>28</v>
       </c>
       <c r="F84" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G84" t="s">
+        <v>306</v>
+      </c>
+      <c r="H84" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>110</v>
+      </c>
+      <c r="F85" t="s">
+        <v>184</v>
+      </c>
+      <c r="G85" t="s">
+        <v>311</v>
+      </c>
+      <c r="H85" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>28</v>
+      </c>
+      <c r="F86" t="s">
+        <v>185</v>
+      </c>
+      <c r="G86" t="s">
+        <v>312</v>
+      </c>
+      <c r="H86" t="s">
         <v>316</v>
-      </c>
-      <c r="H84" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
-        <v>35</v>
+        <v>110</v>
+      </c>
+      <c r="F87" t="s">
+        <v>186</v>
       </c>
       <c r="G87" t="s">
-        <v>162</v>
+        <v>313</v>
       </c>
       <c r="H87" t="s">
-        <v>282</v>
+        <v>317</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
-        <v>112</v>
+        <v>28</v>
       </c>
       <c r="F88" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G88" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="H88" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D89" t="s">
-        <v>28</v>
-      </c>
-      <c r="F89" t="s">
-        <v>191</v>
-      </c>
-      <c r="G89" t="s">
-        <v>322</v>
-      </c>
-      <c r="H89" t="s">
-        <v>326</v>
+      <c r="B89" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D90" t="s">
-        <v>112</v>
-      </c>
-      <c r="F90" t="s">
-        <v>192</v>
-      </c>
-      <c r="G90" t="s">
-        <v>323</v>
-      </c>
-      <c r="H90" t="s">
-        <v>327</v>
+      <c r="B90" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D91" t="s">
-        <v>28</v>
-      </c>
-      <c r="F91" t="s">
-        <v>193</v>
+        <v>35</v>
       </c>
       <c r="G91" t="s">
-        <v>324</v>
+        <v>160</v>
       </c>
       <c r="H91" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D92" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F92" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G92" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="H92" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
@@ -2647,27 +2684,27 @@
         <v>28</v>
       </c>
       <c r="F93" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G93" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="H93" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D94" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F94" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G94" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="H94" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
@@ -2675,127 +2712,133 @@
         <v>28</v>
       </c>
       <c r="F95" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G95" t="s">
+        <v>322</v>
+      </c>
+      <c r="H95" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>110</v>
+      </c>
+      <c r="F96" t="s">
+        <v>192</v>
+      </c>
+      <c r="G96" t="s">
+        <v>327</v>
+      </c>
+      <c r="H96" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>28</v>
+      </c>
+      <c r="F97" t="s">
+        <v>193</v>
+      </c>
+      <c r="G97" t="s">
+        <v>328</v>
+      </c>
+      <c r="H97" t="s">
         <v>332</v>
-      </c>
-      <c r="H95" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D98" t="s">
-        <v>77</v>
-      </c>
-      <c r="E98" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="F98" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G98" t="s">
-        <v>198</v>
+        <v>329</v>
       </c>
       <c r="H98" t="s">
-        <v>279</v>
+        <v>333</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>80</v>
-      </c>
-      <c r="C99" t="s">
-        <v>200</v>
+      <c r="D99" t="s">
+        <v>28</v>
+      </c>
+      <c r="F99" t="s">
+        <v>195</v>
+      </c>
+      <c r="G99" t="s">
+        <v>330</v>
+      </c>
+      <c r="H99" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D100" t="s">
-        <v>112</v>
-      </c>
-      <c r="F100" t="s">
-        <v>201</v>
-      </c>
-      <c r="G100" t="s">
-        <v>202</v>
-      </c>
-      <c r="H100" t="s">
-        <v>280</v>
+      <c r="B100" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>38</v>
+      <c r="D102" t="s">
+        <v>75</v>
+      </c>
+      <c r="E102" t="s">
+        <v>47</v>
+      </c>
+      <c r="F102" t="s">
+        <v>197</v>
+      </c>
+      <c r="G102" t="s">
+        <v>196</v>
+      </c>
+      <c r="H102" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>37</v>
+        <v>78</v>
+      </c>
+      <c r="C103" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
-        <v>35</v>
+        <v>110</v>
+      </c>
+      <c r="F104" t="s">
+        <v>199</v>
       </c>
       <c r="G104" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H104" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D105" t="s">
-        <v>35</v>
-      </c>
-      <c r="G105" t="s">
-        <v>295</v>
-      </c>
-      <c r="H105" t="s">
-        <v>295</v>
+      <c r="B105" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D106" t="s">
-        <v>112</v>
-      </c>
-      <c r="F106" t="s">
-        <v>209</v>
-      </c>
-      <c r="G106" t="s">
-        <v>204</v>
-      </c>
-      <c r="H106" t="s">
-        <v>283</v>
+      <c r="B106" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D107" t="s">
-        <v>28</v>
-      </c>
-      <c r="F107" t="s">
-        <v>208</v>
-      </c>
-      <c r="G107" t="s">
-        <v>205</v>
-      </c>
-      <c r="H107" t="s">
-        <v>284</v>
+      <c r="B107" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.25">
@@ -2803,56 +2846,71 @@
         <v>35</v>
       </c>
       <c r="G108" t="s">
-        <v>294</v>
+        <v>201</v>
       </c>
       <c r="H108" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
-        <v>112</v>
-      </c>
-      <c r="F109" t="s">
-        <v>210</v>
+        <v>35</v>
       </c>
       <c r="G109" t="s">
-        <v>204</v>
+        <v>293</v>
       </c>
       <c r="H109" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
+        <v>110</v>
+      </c>
+      <c r="F110" t="s">
+        <v>207</v>
+      </c>
+      <c r="G110" t="s">
+        <v>202</v>
+      </c>
+      <c r="H110" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
         <v>28</v>
       </c>
-      <c r="F110" t="s">
-        <v>211</v>
-      </c>
-      <c r="G110" t="s">
-        <v>205</v>
-      </c>
-      <c r="H110" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>38</v>
+      <c r="F111" t="s">
+        <v>206</v>
+      </c>
+      <c r="G111" t="s">
+        <v>203</v>
+      </c>
+      <c r="H111" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
-        <v>37</v>
+      <c r="D112" t="s">
+        <v>35</v>
+      </c>
+      <c r="G112" t="s">
+        <v>292</v>
+      </c>
+      <c r="H112" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D113" t="s">
-        <v>35</v>
+        <v>110</v>
+      </c>
+      <c r="F113" t="s">
+        <v>208</v>
       </c>
       <c r="G113" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H113" t="s">
         <v>281</v>
@@ -2860,41 +2918,26 @@
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D114" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="F114" t="s">
+        <v>209</v>
       </c>
       <c r="G114" t="s">
-        <v>293</v>
+        <v>203</v>
       </c>
       <c r="H114" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D115" t="s">
-        <v>112</v>
-      </c>
-      <c r="F115" t="s">
-        <v>212</v>
-      </c>
-      <c r="G115" t="s">
-        <v>204</v>
-      </c>
-      <c r="H115" t="s">
-        <v>283</v>
+      <c r="B115" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D116" t="s">
-        <v>28</v>
-      </c>
-      <c r="F116" t="s">
-        <v>213</v>
-      </c>
-      <c r="G116" t="s">
-        <v>205</v>
-      </c>
-      <c r="H116" t="s">
-        <v>284</v>
+      <c r="B116" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.25">
@@ -2902,384 +2945,434 @@
         <v>35</v>
       </c>
       <c r="G117" t="s">
-        <v>292</v>
+        <v>201</v>
       </c>
       <c r="H117" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>112</v>
-      </c>
-      <c r="F118" t="s">
-        <v>214</v>
+        <v>35</v>
       </c>
       <c r="G118" t="s">
-        <v>204</v>
+        <v>291</v>
       </c>
       <c r="H118" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D119" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="F119" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G119" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H119" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D120" t="s">
-        <v>77</v>
-      </c>
-      <c r="E120" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="F120" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G120" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H120" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
-        <v>80</v>
-      </c>
-      <c r="C121" t="s">
-        <v>218</v>
-      </c>
-      <c r="H121" s="21"/>
+      <c r="D121" t="s">
+        <v>35</v>
+      </c>
+      <c r="G121" t="s">
+        <v>290</v>
+      </c>
+      <c r="H121" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D122" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="F122" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G122" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H122" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="123" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>85</v>
+      <c r="D123" t="s">
+        <v>28</v>
+      </c>
+      <c r="F123" t="s">
+        <v>213</v>
+      </c>
+      <c r="G123" t="s">
+        <v>203</v>
+      </c>
+      <c r="H123" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="124" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B124" t="s">
-        <v>38</v>
+      <c r="D124" t="s">
+        <v>75</v>
+      </c>
+      <c r="E124" t="s">
+        <v>47</v>
+      </c>
+      <c r="F124" t="s">
+        <v>214</v>
+      </c>
+      <c r="G124" t="s">
+        <v>204</v>
+      </c>
+      <c r="H124" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>37</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C125" t="s">
+        <v>216</v>
+      </c>
+      <c r="H125" s="21"/>
     </row>
     <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
-        <v>77</v>
-      </c>
-      <c r="E126" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F126" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G126" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="H126" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>80</v>
-      </c>
-      <c r="C127" t="s">
-        <v>296</v>
+        <v>83</v>
       </c>
     </row>
     <row r="128" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D128" t="s">
-        <v>77</v>
-      </c>
-      <c r="E128" t="s">
-        <v>301</v>
-      </c>
-      <c r="F128" t="s">
-        <v>221</v>
-      </c>
-      <c r="G128" t="s">
-        <v>222</v>
-      </c>
-      <c r="H128" t="s">
-        <v>288</v>
+      <c r="B128" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
+      <c r="D130" t="s">
+        <v>75</v>
+      </c>
+      <c r="E130" t="s">
+        <v>47</v>
+      </c>
+      <c r="F130" t="s">
+        <v>218</v>
+      </c>
+      <c r="G130" t="s">
+        <v>217</v>
+      </c>
+      <c r="H130" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>78</v>
+      </c>
+      <c r="C131" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D132" t="s">
+        <v>75</v>
+      </c>
+      <c r="E132" t="s">
+        <v>299</v>
+      </c>
+      <c r="F132" t="s">
+        <v>219</v>
+      </c>
+      <c r="G132" t="s">
+        <v>220</v>
+      </c>
+      <c r="H132" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D138" t="s">
-        <v>77</v>
-      </c>
-      <c r="E138" t="s">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
+        <v>75</v>
+      </c>
+      <c r="E142" t="s">
         <v>47</v>
       </c>
-      <c r="F138" t="s">
-        <v>247</v>
-      </c>
-      <c r="G138" t="s">
-        <v>299</v>
-      </c>
-      <c r="H138" t="s">
+      <c r="F142" t="s">
+        <v>245</v>
+      </c>
+      <c r="G142" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
-        <v>80</v>
-      </c>
-      <c r="C139" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D140" t="s">
-        <v>45</v>
-      </c>
-      <c r="F140" t="s">
-        <v>249</v>
-      </c>
-      <c r="G140" t="s">
-        <v>207</v>
-      </c>
-      <c r="H140" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D141" t="s">
-        <v>77</v>
-      </c>
-      <c r="E141" t="s">
-        <v>47</v>
-      </c>
-      <c r="F141" t="s">
-        <v>250</v>
-      </c>
-      <c r="G141" t="s">
-        <v>300</v>
-      </c>
-      <c r="H141" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B142" t="s">
-        <v>127</v>
+      <c r="H142" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>38</v>
+        <v>78</v>
+      </c>
+      <c r="C143" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
-        <v>37</v>
+      <c r="D144" t="s">
+        <v>45</v>
+      </c>
+      <c r="F144" t="s">
+        <v>247</v>
+      </c>
+      <c r="G144" t="s">
+        <v>205</v>
+      </c>
+      <c r="H144" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D145" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E145" t="s">
         <v>47</v>
       </c>
       <c r="F145" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="G145" t="s">
-        <v>226</v>
+        <v>298</v>
       </c>
       <c r="H145" t="s">
-        <v>227</v>
+        <v>296</v>
       </c>
     </row>
     <row r="146" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>80</v>
-      </c>
-      <c r="C146" t="s">
-        <v>228</v>
+        <v>125</v>
       </c>
     </row>
     <row r="147" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D147" t="s">
-        <v>45</v>
-      </c>
-      <c r="F147" t="s">
-        <v>229</v>
-      </c>
-      <c r="G147" t="s">
-        <v>207</v>
-      </c>
-      <c r="H147" t="s">
+      <c r="B147" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
+        <v>75</v>
+      </c>
+      <c r="E149" t="s">
+        <v>47</v>
+      </c>
+      <c r="F149" t="s">
+        <v>223</v>
+      </c>
+      <c r="G149" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D148" t="s">
-        <v>45</v>
-      </c>
-      <c r="F148" t="s">
-        <v>230</v>
-      </c>
-      <c r="G148" t="s">
-        <v>231</v>
-      </c>
-      <c r="H148" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B149" t="s">
-        <v>127</v>
+      <c r="H149" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="150" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>38</v>
+        <v>78</v>
+      </c>
+      <c r="C150" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B151" t="s">
-        <v>37</v>
+      <c r="D151" t="s">
+        <v>45</v>
+      </c>
+      <c r="F151" t="s">
+        <v>227</v>
+      </c>
+      <c r="G151" t="s">
+        <v>205</v>
+      </c>
+      <c r="H151" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
-        <v>77</v>
-      </c>
-      <c r="E152" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F152" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="G152" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="H152" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>80</v>
-      </c>
-      <c r="C153" t="s">
-        <v>236</v>
+        <v>125</v>
       </c>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D154" t="s">
-        <v>45</v>
-      </c>
-      <c r="F154" t="s">
-        <v>237</v>
-      </c>
-      <c r="G154" t="s">
-        <v>238</v>
-      </c>
-      <c r="H154" t="s">
-        <v>224</v>
+      <c r="B154" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="155" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
     </row>
     <row r="156" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
-        <v>45</v>
+        <v>75</v>
+      </c>
+      <c r="E156" t="s">
+        <v>47</v>
       </c>
       <c r="F156" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="G156" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="H156" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="157" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D157" t="s">
-        <v>98</v>
-      </c>
-      <c r="F157" t="s">
-        <v>251</v>
-      </c>
-      <c r="G157" t="s">
-        <v>242</v>
-      </c>
-      <c r="H157" t="s">
-        <v>243</v>
+      <c r="B157" t="s">
+        <v>78</v>
+      </c>
+      <c r="C157" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="158" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D158" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="F158" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="G158" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="H158" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
     </row>
     <row r="159" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D160" t="s">
+        <v>45</v>
+      </c>
+      <c r="F160" t="s">
+        <v>237</v>
+      </c>
+      <c r="G160" t="s">
+        <v>238</v>
+      </c>
+      <c r="H160" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
+        <v>96</v>
+      </c>
+      <c r="F161" t="s">
+        <v>249</v>
+      </c>
+      <c r="G161" t="s">
+        <v>240</v>
+      </c>
+      <c r="H161" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D162" t="s">
+        <v>96</v>
+      </c>
+      <c r="F162" t="s">
+        <v>242</v>
+      </c>
+      <c r="G162" t="s">
+        <v>243</v>
+      </c>
+      <c r="H162" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3326,13 +3419,13 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3340,13 +3433,13 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3354,13 +3447,13 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3368,13 +3461,13 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3382,13 +3475,13 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3396,13 +3489,13 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3411,32 +3504,32 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3445,32 +3538,32 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B12" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" t="s">
         <v>107</v>
-      </c>
-      <c r="D12" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B13" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C13" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3567,32 +3660,32 @@
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B22" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C22" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="D22" t="s">
         <v>301</v>
-      </c>
-      <c r="D22" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B23" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>302</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4268,11 +4361,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4298,310 +4391,292 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8"/>
+      <c r="C8" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
       </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
       </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
       </c>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>250</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
       </c>
-      <c r="E13"/>
-      <c r="F13"/>
+      <c r="I13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
       </c>
-      <c r="E14"/>
-      <c r="F14"/>
+      <c r="I14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
       </c>
-      <c r="E15"/>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
       </c>
-      <c r="E17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
       </c>
-      <c r="E18"/>
-      <c r="G18"/>
-    </row>
-    <row r="19" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="E19"/>
+      <c r="F19"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
       </c>
-      <c r="G20"/>
+      <c r="E20"/>
+      <c r="F20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21"/>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
       </c>
-      <c r="G22"/>
+      <c r="D22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
       </c>
-      <c r="G23"/>
+      <c r="E23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
       </c>
+      <c r="E24"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
       </c>
-      <c r="G25"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -4610,97 +4685,101 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
       </c>
-      <c r="E27"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
       </c>
+      <c r="G28"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
       </c>
-      <c r="E29"/>
+      <c r="G29"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
       </c>
+      <c r="G30"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
       </c>
+      <c r="G31"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
         <v>45</v>
@@ -4708,87 +4787,88 @@
       <c r="C35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B43" t="s">
         <v>28</v>
@@ -4797,20 +4877,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B45" t="s">
         <v>28</v>
@@ -4819,20 +4899,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B47" t="s">
         <v>28</v>
@@ -4841,12 +4921,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -4854,7 +4934,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B49" t="s">
         <v>28</v>
@@ -4865,10 +4945,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -4876,7 +4956,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B51" t="s">
         <v>28</v>
@@ -4887,10 +4967,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -4898,10 +4978,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B53" t="s">
-        <v>112</v>
+        <v>28</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -4909,10 +4989,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -4920,7 +5000,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="B55" t="s">
         <v>28</v>
@@ -4931,10 +5011,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -4942,7 +5022,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="B57" t="s">
         <v>28</v>
@@ -4953,10 +5033,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
@@ -4964,10 +5044,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B59" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -4975,10 +5055,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B60" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -4986,7 +5066,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B61" t="s">
         <v>28</v>
@@ -4997,10 +5077,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -5008,10 +5088,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B63" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -5019,10 +5099,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
@@ -5030,10 +5110,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
@@ -5041,10 +5121,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
@@ -5052,10 +5132,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -5063,10 +5143,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>250</v>
+        <v>214</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -5074,10 +5154,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -5085,10 +5165,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="B70" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
@@ -5096,10 +5176,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="B71" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
@@ -5107,10 +5187,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
@@ -5118,7 +5198,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="B73" t="s">
         <v>45</v>
@@ -5129,10 +5209,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="B74" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C74" t="b">
         <v>0</v>
@@ -5140,10 +5220,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="B75" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -5151,18 +5231,85 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="B76" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="C76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>228</v>
+      </c>
+      <c r="B77" t="s">
+        <v>45</v>
+      </c>
+      <c r="C77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>231</v>
+      </c>
+      <c r="B78" t="s">
+        <v>75</v>
+      </c>
+      <c r="C78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>235</v>
+      </c>
+      <c r="B79" t="s">
+        <v>45</v>
+      </c>
+      <c r="C79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>237</v>
+      </c>
+      <c r="B80" t="s">
+        <v>45</v>
+      </c>
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>249</v>
+      </c>
+      <c r="B81" t="s">
+        <v>96</v>
+      </c>
+      <c r="C81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>242</v>
+      </c>
+      <c r="B82" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>